<commit_message>
exploratory cluster analysis: part2
-same remarks as previous push
</commit_message>
<xml_diff>
--- a/_CLUSTER/groups_time_area/groups_counts_area1_J.xlsx
+++ b/_CLUSTER/groups_time_area/groups_counts_area1_J.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -375,10 +375,10 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>125</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3">
@@ -386,23 +386,23 @@
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>116</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" t="n">
-        <v>109</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>102</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6">
@@ -410,47 +410,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="n">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B7" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="n">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B9" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B11" t="n">
-        <v>8</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Looking for trends in Frost classification
-some trends can be seen, especially for area1 and the oldest rock samples
</commit_message>
<xml_diff>
--- a/_CLUSTER/groups_time_area/groups_counts_area1_J.xlsx
+++ b/_CLUSTER/groups_time_area/groups_counts_area1_J.xlsx
@@ -367,10 +367,8 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>groups</t>
-        </is>
+      <c r="B1" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="2">

</xml_diff>